<commit_message>
Pushing latest data updates for database
</commit_message>
<xml_diff>
--- a/data/1_research/research.xlsx
+++ b/data/1_research/research.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\biobib\data\1_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1D8D4E-C6ED-4ABF-9C58-5CF55FC172E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1844C56-1BBE-46B5-86E4-7616767AF340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="209">
   <si>
     <t>N.</t>
   </si>
@@ -603,9 +603,6 @@
     <t>Jason Jon Benedict, Kimberly M. Carlson, Ramada Febrian and Robert Heilmayr</t>
   </si>
   <si>
-    <t>Revise and resubmit</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1017/CBO9781139177245.007</t>
   </si>
   <si>
@@ -615,9 +612,6 @@
     <t>C-1</t>
   </si>
   <si>
-    <t>Climate change poses underappreciated threat to mesic forests</t>
-  </si>
-  <si>
     <t>C-2</t>
   </si>
   <si>
@@ -625,9 +619,6 @@
   </si>
   <si>
     <t>C-4</t>
-  </si>
-  <si>
-    <t>C-5</t>
   </si>
   <si>
     <t>Supply chain governance for sustainability and smallholder
@@ -686,6 +677,12 @@
   </si>
   <si>
     <t>Michael Eggen, Robert Heilmayr, Patrick Anderson, Rebecca Armson, Kemen Austin, Reza Azmi, Peter Bayliss, David Burns, JT Erbaugh, Andini Desita Ekaputri, David Gaveau, Janina Grabs, Aida Greenbury, Ibrahim Gulagnar, Mansuetus Alsy Hanu, Tony Hill, Marieke Leegwater, Godwin Limberg, Charlotte Opal, Violace Putri, Judy Rodrigues, Grant Rosoman, Musnanda Satar, Su Sin Sheun, Uki, Sarah Walen and Kimberly M. Carlson</t>
+  </si>
+  <si>
+    <t>B-38</t>
+  </si>
+  <si>
+    <t>Drought sensitivity in mesic forests heightens their vulnerability to climate change</t>
   </si>
 </sst>
 </file>
@@ -1636,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2052,7 +2049,7 @@
         <v>33</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -3125,7 +3122,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B38">
         <v>2023</v>
@@ -3160,13 +3157,13 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="B39">
         <v>2023</v>
       </c>
       <c r="C39" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="D39" t="s">
         <v>188</v>
@@ -3175,7 +3172,7 @@
         <v>178</v>
       </c>
       <c r="H39" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="I39" t="s">
         <v>15</v>
@@ -3184,7 +3181,7 @@
         <v>4</v>
       </c>
       <c r="K39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -3195,19 +3192,19 @@
     </row>
     <row r="40" spans="1:13" ht="28.8">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D40" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E40" t="s">
         <v>97</v>
       </c>
       <c r="H40" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J40">
         <v>4</v>
@@ -3221,19 +3218,19 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C41" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E41" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H41" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J41">
         <v>4</v>
@@ -3247,19 +3244,19 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E42" t="s">
         <v>97</v>
       </c>
       <c r="H42" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J42">
         <v>4</v>
@@ -3273,19 +3270,19 @@
     </row>
     <row r="43" spans="1:13" ht="86.4">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E43" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H43" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J43">
         <v>4</v>

</xml_diff>